<commit_message>
issue#88 - Table support
</commit_message>
<xml_diff>
--- a/src/test/resources/org/jxls/transform/poi/table.xlsx
+++ b/src/test/resources/org/jxls/transform/poi/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\git-repos\jxls2dev\jxls-poi\src\test\resources\org\jxls\transform\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55D64D6-E341-4CDE-9AB5-62CE3818A058}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399FB322-B545-4E42-BB24-EAB6D18BE3C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{38BEE195-C9BE-4D57-82F8-EA3F59166CB8}"/>
   </bookViews>
@@ -74,7 +74,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="list", var="a", lastCell="B3")</t>
+jx:each(items="list", var="a", table="1", lastCell="B3")</t>
         </r>
       </text>
     </comment>

</xml_diff>